<commit_message>
NOW NOISE COMPARE FILE
</commit_message>
<xml_diff>
--- a/Semantle_AI/Service/Reports_output/Priority_calculation/error_calc_compare.xlsx
+++ b/Semantle_AI/Service/Reports_output/Priority_calculation/error_calc_compare.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bardamri/SE_Project_Semantle/Semantle_AI/Service/Reports_output/Priority_calculation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B55A6CE-90C3-8944-884F-8CCF64C899D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965CEC0E-ADC0-604F-A6B0-D3A94048E6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="27040" windowHeight="16880" xr2:uid="{2BD9F7E4-3864-E14D-AD8C-55EBE9E46C48}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{2BD9F7E4-3864-E14D-AD8C-55EBE9E46C48}"/>
   </bookViews>
   <sheets>
     <sheet name="GLOVE_FASTTEXT" sheetId="2" r:id="rId1"/>
@@ -36,36 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>VALUE</t>
-  </si>
-  <si>
-    <t>SV= SUM_VEC</t>
-  </si>
-  <si>
-    <t>SR = SUM_RELATIVE</t>
-  </si>
-  <si>
-    <t>BF = BRUTE FORCE</t>
-  </si>
-  <si>
-    <t>SR * SV</t>
-  </si>
-  <si>
-    <t>BF * SV</t>
-  </si>
-  <si>
-    <t>SUM * MSE</t>
-  </si>
-  <si>
-    <t>SR * MSE</t>
-  </si>
-  <si>
-    <t>BF * MSE</t>
-  </si>
-  <si>
-    <t>SUM * SV</t>
   </si>
   <si>
     <t>Median</t>
@@ -208,6 +181,27 @@
   <si>
     <t>words</t>
   </si>
+  <si>
+    <t>% מתאים</t>
+  </si>
+  <si>
+    <t>SUM * Mean Squared Error</t>
+  </si>
+  <si>
+    <t>SUM_RELATIVE * Mean Squared Error</t>
+  </si>
+  <si>
+    <t>Brute force  * Mean Squared Error</t>
+  </si>
+  <si>
+    <t>Brute force  * Sum vector</t>
+  </si>
+  <si>
+    <t>Sum relative * Sum vector</t>
+  </si>
+  <si>
+    <t>SUM * Sum vec</t>
+  </si>
 </sst>
 </file>
 
@@ -273,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -281,12 +275,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -439,22 +435,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>SUM * SV</c:v>
+                  <c:v>SUM * Sum vec</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SR * SV</c:v>
+                  <c:v>Sum relative * Sum vector</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>BF * SV</c:v>
+                  <c:v>Brute force  * Sum vector</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>SUM * MSE</c:v>
+                  <c:v>SUM * Mean Squared Error</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>SR * MSE</c:v>
+                  <c:v>SUM_RELATIVE * Mean Squared Error</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>BF * MSE</c:v>
+                  <c:v>Brute force  * Mean Squared Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -881,22 +877,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>SUM * SV</c:v>
+                  <c:v>SUM * Sum vec</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SR * SV</c:v>
+                  <c:v>Sum relative * Sum vector</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>BF * SV</c:v>
+                  <c:v>Brute force  * Sum vector</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>SUM * MSE</c:v>
+                  <c:v>SUM * Mean Squared Error</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>SR * MSE</c:v>
+                  <c:v>SUM_RELATIVE * Mean Squared Error</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>BF * MSE</c:v>
+                  <c:v>Brute force  * Mean Squared Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1245,22 +1241,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>SUM * SV</c:v>
+                  <c:v>SUM * Sum vec</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SR * SV</c:v>
+                  <c:v>Sum relative * Sum vector</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>BF * SV</c:v>
+                  <c:v>Brute force  * Sum vector</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>SUM * MSE</c:v>
+                  <c:v>SUM * Mean Squared Error</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>SR * MSE</c:v>
+                  <c:v>SUM_RELATIVE * Mean Squared Error</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>BF * MSE</c:v>
+                  <c:v>Brute force  * Mean Squared Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1628,22 +1624,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>SUM * SV</c:v>
+                  <c:v>SUM * Sum vec</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>SR * SV</c:v>
+                  <c:v>Sum relative * Sum vector</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>BF * SV</c:v>
+                  <c:v>Brute force  * Sum vector</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>SUM * MSE</c:v>
+                  <c:v>SUM * Mean Squared Error</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>SR * MSE</c:v>
+                  <c:v>SUM_RELATIVE * Mean Squared Error</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>BF * MSE</c:v>
+                  <c:v>Brute force  * Mean Squared Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4146,16 +4142,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>804333</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>8467</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>422209</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>30946</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1041401</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>142286</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>124079</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4184,16 +4180,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1041400</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>108569</xdr:colOff>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>194733</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>728134</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>84667</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>537073</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>84668</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4222,16 +4218,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>804333</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>93133</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>377254</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>171806</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1035050</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>177799</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>293281</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>54171</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4260,16 +4256,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1024466</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>788449</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>22928</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>694266</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>379576</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>199828</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4300,17 +4296,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FA48D039-1206-FD4C-B2C7-86CE32119496}" name="Table13" displayName="Table13" ref="H7:N13" totalsRowShown="0">
-  <autoFilter ref="H7:N13" xr:uid="{FA48D039-1206-FD4C-B2C7-86CE32119496}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FA48D039-1206-FD4C-B2C7-86CE32119496}" name="Table13" displayName="Table13" ref="H7:O13" totalsRowShown="0">
+  <autoFilter ref="H7:O13" xr:uid="{FA48D039-1206-FD4C-B2C7-86CE32119496}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{24B8A575-2FD5-A246-9280-8A2516EBA594}" name="VALUE"/>
-    <tableColumn id="2" xr3:uid="{D0542DFB-E232-864E-B4A0-2F325C3ECAF4}" name="Average" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{D0542DFB-E232-864E-B4A0-2F325C3ECAF4}" name="Average" dataDxfId="6">
       <calculatedColumnFormula>AVERAGE(A2:A501)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FE3C593F-B1CD-3648-AE12-303DDDA814D1}" name="Median" dataDxfId="4">
+    <tableColumn id="3" xr3:uid="{FE3C593F-B1CD-3648-AE12-303DDDA814D1}" name="Median" dataDxfId="5">
       <calculatedColumnFormula>MEDIAN(B1:B1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0176FEAF-7914-1C41-AA24-790D0CF2B04B}" name="Variance" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{0176FEAF-7914-1C41-AA24-790D0CF2B04B}" name="Variance" dataDxfId="4">
       <calculatedColumnFormula>VAR(A2:A501)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{B7A74FC3-444B-C84C-98F5-69A570F6B02C}" name="STANDARD DEVIATION" dataDxfId="3">
@@ -4322,6 +4318,7 @@
     <tableColumn id="8" xr3:uid="{0B28689D-C1F4-4D4C-95B1-6701E925779D}" name="MAX VALUE" dataDxfId="1">
       <calculatedColumnFormula>MAX(B1:B500)</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="5" xr3:uid="{2165A3A0-F56E-D842-BC2A-02718C45041C}" name="% מתאים" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4624,14 +4621,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08AAC9F3-9758-EE4C-9725-9BEBC9FEF52E}">
-  <dimension ref="A1:N1001"/>
+  <dimension ref="A1:O1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="S45" sqref="S45"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.1640625" customWidth="1"/>
@@ -4639,34 +4639,30 @@
     <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="4"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>4103</v>
       </c>
@@ -4686,14 +4682,10 @@
         <v>321</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2121</v>
       </c>
@@ -4713,14 +4705,10 @@
         <v>913</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2411</v>
       </c>
@@ -4740,10 +4728,12 @@
         <v>1236</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2662</v>
       </c>
@@ -4763,10 +4753,12 @@
         <v>2535</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2459</v>
       </c>
@@ -4786,10 +4778,12 @@
         <v>3998</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2198</v>
       </c>
@@ -4809,31 +4803,34 @@
         <v>3562</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="J7" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="M7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="N7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="O7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>711</v>
       </c>
@@ -4853,11 +4850,11 @@
         <v>1540</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H8" t="str">
         <f>A1</f>
-        <v>SUM * SV</v>
+        <v>SUM * Sum vec</v>
       </c>
       <c r="I8">
         <f>AVERAGE(A2:A501)</f>
@@ -4883,8 +4880,11 @@
         <f>MAX(A2:A501)</f>
         <v>4106</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2160</v>
       </c>
@@ -4904,11 +4904,11 @@
         <v>2191</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H9" t="str">
         <f>B1</f>
-        <v>SR * SV</v>
+        <v>Sum relative * Sum vector</v>
       </c>
       <c r="I9">
         <f>AVERAGE(B2:B501)</f>
@@ -4934,8 +4934,11 @@
         <f>MAX(B2:B501)</f>
         <v>4145</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>3946</v>
       </c>
@@ -4955,11 +4958,11 @@
         <v>609</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H10" t="str">
         <f>C1</f>
-        <v>BF * SV</v>
+        <v>Brute force  * Sum vector</v>
       </c>
       <c r="I10">
         <f>AVERAGE(C2:C501)</f>
@@ -4986,7 +4989,7 @@
         <v>3860</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>88</v>
       </c>
@@ -5006,11 +5009,11 @@
         <v>2743</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H11" t="str">
         <f>D1</f>
-        <v>SUM * MSE</v>
+        <v>SUM * Mean Squared Error</v>
       </c>
       <c r="I11">
         <f>AVERAGE(D2:D501)</f>
@@ -5036,8 +5039,11 @@
         <f>MAX(D2:D501)</f>
         <v>4010</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>912</v>
       </c>
@@ -5057,11 +5063,11 @@
         <v>3470</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H12" t="str">
         <f>E1</f>
-        <v>SR * MSE</v>
+        <v>SUM_RELATIVE * Mean Squared Error</v>
       </c>
       <c r="I12">
         <f>AVERAGE(E2:E501)</f>
@@ -5088,7 +5094,7 @@
         <v>4119</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>3801</v>
       </c>
@@ -5108,11 +5114,11 @@
         <v>3688</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H13" t="str">
         <f>F1</f>
-        <v>BF * MSE</v>
+        <v>Brute force  * Mean Squared Error</v>
       </c>
       <c r="I13">
         <f>AVERAGE(F2:F501)</f>
@@ -5139,7 +5145,7 @@
         <v>4163</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1988</v>
       </c>
@@ -5159,10 +5165,10 @@
         <v>4163</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>3923</v>
       </c>
@@ -5182,10 +5188,10 @@
         <v>3308</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1571</v>
       </c>
@@ -5205,7 +5211,7 @@
         <v>3708</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -5228,7 +5234,7 @@
         <v>403</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -5251,7 +5257,7 @@
         <v>2197</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -5274,7 +5280,7 @@
         <v>3816</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -5297,7 +5303,7 @@
         <v>633</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -5320,7 +5326,7 @@
         <v>2301</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -5343,7 +5349,7 @@
         <v>192</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -5366,7 +5372,7 @@
         <v>1412</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -5389,7 +5395,7 @@
         <v>1957</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -5412,7 +5418,7 @@
         <v>43</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -5435,7 +5441,7 @@
         <v>1700</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -5458,7 +5464,7 @@
         <v>1689</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -5481,7 +5487,7 @@
         <v>386</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -5504,7 +5510,7 @@
         <v>2498</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -5527,7 +5533,7 @@
         <v>601</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -5550,7 +5556,7 @@
         <v>2313</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -5573,7 +5579,7 @@
         <v>702</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -5596,7 +5602,7 @@
         <v>2664</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -5619,7 +5625,7 @@
         <v>2794</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -5642,7 +5648,7 @@
         <v>2756</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -5665,7 +5671,7 @@
         <v>2530</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -5688,7 +5694,7 @@
         <v>3487</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -5711,7 +5717,7 @@
         <v>193</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -5734,7 +5740,7 @@
         <v>517</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -5757,7 +5763,7 @@
         <v>905</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -5780,7 +5786,7 @@
         <v>2739</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -13465,9 +13471,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>